<commit_message>
Various tech edits, update education (subject/focus), add father education example, update mappings, add note to commenters
</commit_message>
<xml_diff>
--- a/input/mapping/BFDR_Profile_Intros.xlsx
+++ b/input/mapping/BFDR_Profile_Intros.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Dropbox\12_SourceControl\GitHub\HL7\FHIR\fhir-bfdr\input\mapping\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Dropbox\12_SourceControl\GitHub\HL7\FHIR\vr-common-library\input\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A358729-D2FD-4721-98CD-1FA05CE55BDE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B12C70-0167-4C2A-B902-0935B84298C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
+    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="163">
   <si>
     <t>Bundle-document-bfdr</t>
   </si>
@@ -539,9 +539,6 @@
     <t>This profile is based on the [US Core RelatedPerson]({{site.data.fhir.ver.hl7fhiruscore}}/StructureDefinition-us-core-relatedperson.html) profile.</t>
   </si>
   <si>
-    <t>This Observation profile represents the number of fetuses delivered live or dead at any time in the pregnancy regardless of gestational age, or if the fetuses were delivered at different dates in the pregnancy. ('Reabsorbed' fetuses, those which are not 'delivered' (expulsed or extracted from the mother) should not be counted.) Include all live births and fetal losses resulting from this pregnancy. This profile represents plurality as a characteristic of the pregnancy. For plurality as a characteristic of the patient, see the Patient.multipleBirth\[x]patient-multipleBirthTotal extension.</t>
-  </si>
-  <si>
     <t>This profile adds further constraints to the [US Core Patient]({{site.data.fhir.ver.hl7fhiruscore}}/StructureDefinition-us-core-patient.html) such as:
 * the [patient-birthPlace](http://hl7.org/fhir/StructureDefinition/patient-birthPlace) extension
 * the [patient-birthTime](http://hl7.org/fhir/StructureDefinition/patient-birthTime) extension
@@ -551,6 +548,10 @@
   </si>
   <si>
     <t>This includes infections present at the start of pregnancy or confirmed diagnosis during pregnancy with or without documentation of treatment. Documentation of treatment during this pregnancy is adequate if a definitive diagnosis is not present in the available record.</t>
+  </si>
+  <si>
+    <t>('Reabsorbed' fetuses, those which are not 'delivered' [expulsed or extracted from the mother] should not be counted.) Include all live births and fetal losses resulting from this pregnancy. 
+This profile represents plurality as a characteristic of the pregnancy. For plurality as a characteristic of the patient, see the [patient-multipleBirthTotal extension](http://hl7.org/fhir/StructureDefinition-patient-multipleBirthTotal.html).</t>
   </si>
 </sst>
 </file>
@@ -921,15 +922,15 @@
   <dimension ref="A1:E138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A8" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B15" sqref="B15"/>
+      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
   <cols>
     <col min="1" max="1" width="55.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.62890625" style="3" customWidth="1"/>
-    <col min="3" max="3" width="12.05078125" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.578125" style="3" customWidth="1"/>
+    <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="10.41796875" style="2" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="13.41796875" style="2" bestFit="1" customWidth="1"/>
     <col min="6" max="16384" width="8.83984375" style="2"/>
@@ -1115,7 +1116,7 @@
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>150</v>
@@ -2436,9 +2437,6 @@
       <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
-      <c r="B118" s="3" t="s">
-        <v>157</v>
-      </c>
       <c r="C118" s="2" t="s">
         <v>150</v>
       </c>
@@ -2454,7 +2452,7 @@
         <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>138</v>
@@ -2537,7 +2535,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>150</v>

</xml_diff>

<commit_message>
Update mapping spreadsheet, mapping scripts, mappings
</commit_message>
<xml_diff>
--- a/input/mapping/BFDR_Profile_Intros.xlsx
+++ b/input/mapping/BFDR_Profile_Intros.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26731"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Dropbox\12_SourceControl\GitHub\HL7\FHIR\vr-common-library\input\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8B12C70-0167-4C2A-B902-0935B84298C3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CDB6B98-C932-4B89-814A-634A93776FF8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-96" yWindow="-96" windowWidth="23232" windowHeight="13992" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
+    <workbookView xWindow="38280" yWindow="-345" windowWidth="29040" windowHeight="15840" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="494" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="163">
   <si>
     <t>Bundle-document-bfdr</t>
   </si>
@@ -922,21 +922,21 @@
   <dimension ref="A1:E138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B119" sqref="B119"/>
+      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C129" sqref="C129"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.83984375" defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="55.83984375" style="2" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="90.578125" style="3" customWidth="1"/>
+    <col min="1" max="1" width="55.85546875" style="2" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="90.5703125" style="3" customWidth="1"/>
     <col min="3" max="3" width="12" style="2" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.41796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="13.41796875" style="2" bestFit="1" customWidth="1"/>
-    <col min="6" max="16384" width="8.83984375" style="2"/>
+    <col min="4" max="4" width="10.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="2" bestFit="1" customWidth="1"/>
+    <col min="6" max="16384" width="8.85546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>145</v>
       </c>
@@ -953,7 +953,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
@@ -961,7 +961,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="3" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="3" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A3" s="2" t="s">
         <v>1</v>
       </c>
@@ -972,7 +972,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="4" spans="1:5" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
         <v>2</v>
       </c>
@@ -983,7 +983,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="5" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
         <v>3</v>
       </c>
@@ -994,7 +994,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="6" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="6" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
         <v>4</v>
       </c>
@@ -1005,7 +1005,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="403.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:5" ht="409.5" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
         <v>5</v>
       </c>
@@ -1016,7 +1016,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="8" spans="1:5" ht="302.39999999999998" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:5" ht="315" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>6</v>
       </c>
@@ -1027,7 +1027,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A9" s="2" t="s">
         <v>7</v>
       </c>
@@ -1041,7 +1041,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A10" s="2" t="s">
         <v>8</v>
       </c>
@@ -1052,7 +1052,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
         <v>9</v>
       </c>
@@ -1063,7 +1063,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
         <v>10</v>
       </c>
@@ -1077,7 +1077,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1094,7 +1094,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1111,7 +1111,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="43.2" x14ac:dyDescent="0.55000000000000004">
+    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
@@ -1128,7 +1128,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A16" s="2" t="s">
         <v>14</v>
       </c>
@@ -1142,7 +1142,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A17" s="2" t="s">
         <v>15</v>
       </c>
@@ -1156,7 +1156,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A18" s="2" t="s">
         <v>16</v>
       </c>
@@ -1170,7 +1170,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A19" s="2" t="s">
         <v>17</v>
       </c>
@@ -1184,29 +1184,41 @@
         <v>74</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A20" s="2" t="s">
         <v>18</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>153</v>
       </c>
+      <c r="C20" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="E20" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
       <c r="B21" s="3" t="s">
         <v>154</v>
       </c>
+      <c r="C21" s="2" t="s">
+        <v>150</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>150</v>
+      </c>
       <c r="E21" s="2" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A22" s="2" t="s">
         <v>20</v>
       </c>
@@ -1220,7 +1232,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A23" s="2" t="s">
         <v>21</v>
       </c>
@@ -1234,7 +1246,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A24" s="2" t="s">
         <v>22</v>
       </c>
@@ -1242,7 +1254,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A25" s="2" t="s">
         <v>23</v>
       </c>
@@ -1256,7 +1268,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A26" s="2" t="s">
         <v>24</v>
       </c>
@@ -1270,7 +1282,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A27" s="2" t="s">
         <v>25</v>
       </c>
@@ -1284,7 +1296,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A28" s="2" t="s">
         <v>26</v>
       </c>
@@ -1298,7 +1310,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A29" s="2" t="s">
         <v>27</v>
       </c>
@@ -1306,7 +1318,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A30" s="2" t="s">
         <v>28</v>
       </c>
@@ -1320,7 +1332,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A31" s="2" t="s">
         <v>29</v>
       </c>
@@ -1334,7 +1346,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A32" s="2" t="s">
         <v>30</v>
       </c>
@@ -1348,7 +1360,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="2" t="s">
         <v>31</v>
       </c>
@@ -1362,7 +1374,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="2" t="s">
         <v>32</v>
       </c>
@@ -1376,7 +1388,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="2" t="s">
         <v>33</v>
       </c>
@@ -1390,7 +1402,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1404,7 +1416,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -1418,7 +1430,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -1432,7 +1444,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -1446,7 +1458,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -1460,7 +1472,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -1474,7 +1486,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -1488,7 +1500,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -1502,7 +1514,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
@@ -1516,7 +1528,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -1530,7 +1542,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -1544,7 +1556,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="57.6" x14ac:dyDescent="0.55000000000000004">
+    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -1558,7 +1570,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="48" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="2" t="s">
         <v>46</v>
       </c>
@@ -1572,7 +1584,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="49" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="2" t="s">
         <v>47</v>
       </c>
@@ -1586,7 +1598,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="50" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="2" t="s">
         <v>48</v>
       </c>
@@ -1600,7 +1612,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="51" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="2" t="s">
         <v>49</v>
       </c>
@@ -1614,7 +1626,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="52" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="2" t="s">
         <v>50</v>
       </c>
@@ -1628,7 +1640,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="53" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="2" t="s">
         <v>51</v>
       </c>
@@ -1642,7 +1654,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="54" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="2" t="s">
         <v>52</v>
       </c>
@@ -1656,7 +1668,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="55" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="2" t="s">
         <v>53</v>
       </c>
@@ -1670,7 +1682,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="56" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="2" t="s">
         <v>54</v>
       </c>
@@ -1684,7 +1696,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="57" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="2" t="s">
         <v>55</v>
       </c>
@@ -1698,7 +1710,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="58" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="2" t="s">
         <v>56</v>
       </c>
@@ -1712,7 +1724,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="59" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="2" t="s">
         <v>57</v>
       </c>
@@ -1726,7 +1738,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="60" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="2" t="s">
         <v>58</v>
       </c>
@@ -1740,7 +1752,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="61" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="2" t="s">
         <v>59</v>
       </c>
@@ -1754,7 +1766,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="62" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="2" t="s">
         <v>60</v>
       </c>
@@ -1768,7 +1780,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="63" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="2" t="s">
         <v>61</v>
       </c>
@@ -1782,7 +1794,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="64" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="2" t="s">
         <v>62</v>
       </c>
@@ -1796,7 +1808,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="65" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="2" t="s">
         <v>63</v>
       </c>
@@ -1810,7 +1822,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="66" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A66" s="2" t="s">
         <v>64</v>
       </c>
@@ -1824,7 +1836,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="67" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A67" s="2" t="s">
         <v>65</v>
       </c>
@@ -1838,7 +1850,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="68" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A68" s="2" t="s">
         <v>66</v>
       </c>
@@ -1852,7 +1864,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="69" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A69" s="2" t="s">
         <v>67</v>
       </c>
@@ -1866,7 +1878,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="70" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A70" s="2" t="s">
         <v>68</v>
       </c>
@@ -1880,7 +1892,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="71" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A71" s="2" t="s">
         <v>69</v>
       </c>
@@ -1894,7 +1906,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="72" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A72" s="2" t="s">
         <v>70</v>
       </c>
@@ -1908,7 +1920,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="73" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A73" s="2" t="s">
         <v>71</v>
       </c>
@@ -1922,7 +1934,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="74" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A74" s="2" t="s">
         <v>72</v>
       </c>
@@ -1936,7 +1948,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="75" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A75" s="2" t="s">
         <v>73</v>
       </c>
@@ -1950,7 +1962,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="76" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="76" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A76" s="2" t="s">
         <v>75</v>
       </c>
@@ -1964,7 +1976,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="77" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="77" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A77" s="2" t="s">
         <v>76</v>
       </c>
@@ -1978,7 +1990,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="78" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="78" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A78" s="2" t="s">
         <v>77</v>
       </c>
@@ -1992,7 +2004,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="79" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="79" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A79" s="2" t="s">
         <v>78</v>
       </c>
@@ -2006,7 +2018,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="80" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="80" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A80" s="2" t="s">
         <v>79</v>
       </c>
@@ -2020,7 +2032,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="81" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="81" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A81" s="2" t="s">
         <v>80</v>
       </c>
@@ -2028,7 +2040,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A82" s="2" t="s">
         <v>81</v>
       </c>
@@ -2036,7 +2048,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="83" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A83" s="2" t="s">
         <v>82</v>
       </c>
@@ -2044,7 +2056,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A84" s="2" t="s">
         <v>83</v>
       </c>
@@ -2052,7 +2064,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="85" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="85" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A85" s="2" t="s">
         <v>84</v>
       </c>
@@ -2060,7 +2072,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="86" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="86" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A86" s="2" t="s">
         <v>85</v>
       </c>
@@ -2068,7 +2080,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="87" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="87" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A87" s="2" t="s">
         <v>86</v>
       </c>
@@ -2076,7 +2088,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A88" s="2" t="s">
         <v>87</v>
       </c>
@@ -2084,7 +2096,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A89" s="2" t="s">
         <v>88</v>
       </c>
@@ -2098,7 +2110,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A90" s="2" t="s">
         <v>89</v>
       </c>
@@ -2106,7 +2118,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A91" s="2" t="s">
         <v>90</v>
       </c>
@@ -2114,7 +2126,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="92" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="92" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A92" s="2" t="s">
         <v>91</v>
       </c>
@@ -2128,7 +2140,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="93" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="93" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A93" s="2" t="s">
         <v>92</v>
       </c>
@@ -2136,7 +2148,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="94" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="94" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A94" s="2" t="s">
         <v>93</v>
       </c>
@@ -2144,7 +2156,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="95" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
@@ -2161,7 +2173,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="96" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="96" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A96" s="2" t="s">
         <v>95</v>
       </c>
@@ -2175,7 +2187,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="97" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="97" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A97" s="2" t="s">
         <v>96</v>
       </c>
@@ -2189,7 +2201,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="98" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="98" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A98" s="2" t="s">
         <v>97</v>
       </c>
@@ -2197,7 +2209,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="99" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="99" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A99" s="2" t="s">
         <v>98</v>
       </c>
@@ -2205,7 +2217,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="100" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="100" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A100" s="2" t="s">
         <v>99</v>
       </c>
@@ -2213,7 +2225,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="101" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="101" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A101" s="2" t="s">
         <v>100</v>
       </c>
@@ -2221,7 +2233,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="102" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="102" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A102" s="2" t="s">
         <v>101</v>
       </c>
@@ -2235,7 +2247,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="103" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="103" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A103" s="2" t="s">
         <v>102</v>
       </c>
@@ -2249,7 +2261,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="104" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="104" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A104" s="2" t="s">
         <v>103</v>
       </c>
@@ -2257,7 +2269,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="105" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="105" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A105" s="2" t="s">
         <v>104</v>
       </c>
@@ -2271,7 +2283,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="106" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="106" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A106" s="2" t="s">
         <v>105</v>
       </c>
@@ -2279,7 +2291,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="107" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="107" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A107" s="2" t="s">
         <v>106</v>
       </c>
@@ -2293,7 +2305,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="108" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="108" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A108" s="2" t="s">
         <v>107</v>
       </c>
@@ -2307,7 +2319,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="109" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="109" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A109" s="2" t="s">
         <v>108</v>
       </c>
@@ -2321,7 +2333,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="110" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="110" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A110" s="2" t="s">
         <v>109</v>
       </c>
@@ -2335,7 +2347,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="111" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="111" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A111" s="2" t="s">
         <v>110</v>
       </c>
@@ -2349,7 +2361,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="112" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="112" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A112" s="2" t="s">
         <v>111</v>
       </c>
@@ -2363,7 +2375,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="113" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="113" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A113" s="2" t="s">
         <v>112</v>
       </c>
@@ -2377,7 +2389,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="114" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="114" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A114" s="2" t="s">
         <v>113</v>
       </c>
@@ -2391,7 +2403,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="115" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="115" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A115" s="2" t="s">
         <v>114</v>
       </c>
@@ -2405,7 +2417,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="116" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="116" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A116" s="2" t="s">
         <v>115</v>
       </c>
@@ -2419,7 +2431,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="117" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="117" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A117" s="2" t="s">
         <v>116</v>
       </c>
@@ -2433,7 +2445,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="118" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="118" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A118" s="2" t="s">
         <v>117</v>
       </c>
@@ -2447,7 +2459,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="86.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="119" spans="1:5" ht="90" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>118</v>
       </c>
@@ -2458,7 +2470,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="120" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="120" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A120" s="2" t="s">
         <v>119</v>
       </c>
@@ -2472,7 +2484,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="121" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="121" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A121" s="2" t="s">
         <v>120</v>
       </c>
@@ -2486,7 +2498,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="100.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="122" spans="1:5" ht="135" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>121</v>
       </c>
@@ -2500,7 +2512,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="123" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>122</v>
       </c>
@@ -2514,7 +2526,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="124" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="124" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A124" s="2" t="s">
         <v>123</v>
       </c>
@@ -2522,7 +2534,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="125" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="125" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A125" s="2" t="s">
         <v>124</v>
       </c>
@@ -2530,7 +2542,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="126" spans="1:5" ht="158.4" x14ac:dyDescent="0.55000000000000004">
+    <row r="126" spans="1:5" ht="180" x14ac:dyDescent="0.25">
       <c r="A126" s="2" t="s">
         <v>125</v>
       </c>
@@ -2547,7 +2559,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="127" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="127" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A127" s="2" t="s">
         <v>126</v>
       </c>
@@ -2561,7 +2573,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="128" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="128" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A128" s="2" t="s">
         <v>127</v>
       </c>
@@ -2575,7 +2587,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="129" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="129" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A129" s="2" t="s">
         <v>128</v>
       </c>
@@ -2589,7 +2601,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="130" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="130" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A130" s="2" t="s">
         <v>129</v>
       </c>
@@ -2603,7 +2615,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="131" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="131" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A131" s="2" t="s">
         <v>130</v>
       </c>
@@ -2617,7 +2629,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="132" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="132" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A132" s="2" t="s">
         <v>131</v>
       </c>
@@ -2625,7 +2637,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="133" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="133" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A133" s="2" t="s">
         <v>132</v>
       </c>
@@ -2639,7 +2651,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="134" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="134" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A134" s="2" t="s">
         <v>133</v>
       </c>
@@ -2653,7 +2665,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="135" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="135" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A135" s="2" t="s">
         <v>134</v>
       </c>
@@ -2661,7 +2673,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="136" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="136" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
@@ -2675,7 +2687,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="137" spans="1:5" x14ac:dyDescent="0.55000000000000004">
+    <row r="137" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A137" s="2" t="s">
         <v>136</v>
       </c>
@@ -2683,7 +2695,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="28.8" x14ac:dyDescent="0.55000000000000004">
+    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>137</v>
       </c>

</xml_diff>

<commit_message>
Remove spurious mapping file, update mapping
</commit_message>
<xml_diff>
--- a/input/mapping/BFDR_Profile_Intros.xlsx
+++ b/input/mapping/BFDR_Profile_Intros.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Dropbox\12_SourceControl\GitHub\HL7\FHIR\vr-common-library\input\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{243A8821-8118-4EA5-9B16-1754D50EBD67}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8AE1B5-4807-4C39-A997-2F851AC4E8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="-345" windowWidth="29040" windowHeight="15840" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="498" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="163">
   <si>
     <t>Bundle-document-bfdr</t>
   </si>
@@ -922,8 +922,8 @@
   <dimension ref="A1:E138"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A122" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B126" sqref="B126"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2677,12 +2677,6 @@
       <c r="A136" s="2" t="s">
         <v>135</v>
       </c>
-      <c r="C136" s="2" t="s">
-        <v>150</v>
-      </c>
-      <c r="D136" s="2" t="s">
-        <v>150</v>
-      </c>
       <c r="E136" s="2" t="s">
         <v>138</v>
       </c>

</xml_diff>

<commit_message>
Update mappings, update profiles based on jiras
</commit_message>
<xml_diff>
--- a/input/mapping/BFDR_Profile_Intros.xlsx
+++ b/input/mapping/BFDR_Profile_Intros.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\minigrrl\Dropbox\12_SourceControl\GitHub\HL7\FHIR\vr-common-library\input\mapping\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC8AE1B5-4807-4C39-A997-2F851AC4E8A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F96A2FA4-A877-4EC8-BC78-38CB196FA6AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21240" xr2:uid="{A8075592-22BD-4EA0-88A4-9AD2EBB5635C}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="496" uniqueCount="163">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="495" uniqueCount="162">
   <si>
     <t>Bundle-document-bfdr</t>
   </si>
@@ -529,13 +529,6 @@
     <t>Birth certificates only require 5 and 10 minute timings. Other use cases may require/accept other timings.</t>
   </si>
   <si>
-    <t>When the Observation is about the father, set the subject to the child and the focus to the father (RelatedPerson).</t>
-  </si>
-  <si>
-    <t>When the Observation is about the father, set the subject to the child and the focus to the father (RelatedPerson).
-In cases where multiple races are recorded for a person an algorithm (NCHS defined) is used to select a single race. The goal is to provide race statistics that are comparable with those used historically to facilitate time series analysis. The goal is to maintain consistency between data collected after the definitional change (allowing collection of multiple races and ethnicities) and that collected prior to that time. This intent is to maintain the integrity of time series (data collected from a range of time periods) reporting.</t>
-  </si>
-  <si>
     <t>This profile is based on the [US Core RelatedPerson]({{site.data.fhir.ver.hl7fhiruscore}}/StructureDefinition-us-core-relatedperson.html) profile.</t>
   </si>
   <si>
@@ -552,6 +545,9 @@
  * the [patient-multipleBirthTotal](http://hl7.org/fhir/StructureDefinition/patient-multipleBirthTotal) extension to record plurality
  * the base FHIR [data-absent-reason](http://hl7.org/fhir/StructureDefinition/data-absent-reason) extension to both name.given and name.family (a name may not yet have been chosen for the baby and US Core Patient requires that Patient.name.given or Patient.name.family or both SHALL be present)
     * use not-applicable if the name hasn't been chosen</t>
+  </si>
+  <si>
+    <t>In cases where multiple races are recorded for a person an algorithm (NCHS defined) is used to select a single race. The goal is to provide race statistics that are comparable with those used historically to facilitate time series analysis. The goal is to maintain consistency between data collected after the definitional change (allowing collection of multiple races and ethnicities) and that collected prior to that time. This intent is to maintain the integrity of time series (data collected from a range of time periods) reporting.</t>
   </si>
 </sst>
 </file>
@@ -923,7 +919,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D79" sqref="D79"/>
+      <selection pane="bottomLeft" activeCell="B4" sqref="B4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1077,7 +1073,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="13" spans="1:5" ht="75" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
         <v>11</v>
       </c>
@@ -1094,7 +1090,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
         <v>12</v>
       </c>
@@ -1111,12 +1107,12 @@
         <v>74</v>
       </c>
     </row>
-    <row r="15" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:5" ht="30" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
         <v>13</v>
       </c>
       <c r="B15" s="3" t="s">
-        <v>160</v>
+        <v>158</v>
       </c>
       <c r="C15" s="2" t="s">
         <v>150</v>
@@ -1201,7 +1197,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="21" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A21" s="2" t="s">
         <v>19</v>
       </c>
@@ -1402,7 +1398,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="36" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A36" s="2" t="s">
         <v>34</v>
       </c>
@@ -1416,7 +1412,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="37" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A37" s="2" t="s">
         <v>35</v>
       </c>
@@ -1430,7 +1426,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="38" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A38" s="2" t="s">
         <v>36</v>
       </c>
@@ -1444,7 +1440,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="39" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A39" s="2" t="s">
         <v>37</v>
       </c>
@@ -1458,7 +1454,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="40" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A40" s="2" t="s">
         <v>38</v>
       </c>
@@ -1472,7 +1468,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="41" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A41" s="2" t="s">
         <v>39</v>
       </c>
@@ -1486,7 +1482,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="42" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A42" s="2" t="s">
         <v>40</v>
       </c>
@@ -1500,7 +1496,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="43" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A43" s="2" t="s">
         <v>41</v>
       </c>
@@ -1514,7 +1510,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="44" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A44" s="2" t="s">
         <v>42</v>
       </c>
@@ -1528,7 +1524,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="45" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A45" s="2" t="s">
         <v>43</v>
       </c>
@@ -1542,7 +1538,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="46" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A46" s="2" t="s">
         <v>44</v>
       </c>
@@ -1556,7 +1552,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="47" spans="1:5" ht="60" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:5" ht="45" x14ac:dyDescent="0.25">
       <c r="A47" s="2" t="s">
         <v>45</v>
       </c>
@@ -2156,7 +2152,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="95" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A95" s="2" t="s">
         <v>94</v>
       </c>
@@ -2459,12 +2455,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="119" spans="1:5" ht="90" x14ac:dyDescent="0.25">
+    <row r="119" spans="1:5" ht="75" x14ac:dyDescent="0.25">
       <c r="A119" s="2" t="s">
         <v>118</v>
       </c>
       <c r="B119" s="3" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="E119" s="2" t="s">
         <v>138</v>
@@ -2498,12 +2494,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="122" spans="1:5" ht="135" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:5" ht="60" x14ac:dyDescent="0.25">
       <c r="A122" s="2" t="s">
         <v>121</v>
       </c>
       <c r="B122" s="3" t="s">
-        <v>158</v>
+        <v>161</v>
       </c>
       <c r="D122" s="2" t="s">
         <v>150</v>
@@ -2512,12 +2508,9 @@
         <v>138</v>
       </c>
     </row>
-    <row r="123" spans="1:5" ht="30" x14ac:dyDescent="0.25">
+    <row r="123" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A123" s="2" t="s">
         <v>122</v>
-      </c>
-      <c r="B123" s="3" t="s">
-        <v>157</v>
       </c>
       <c r="D123" s="2" t="s">
         <v>150</v>
@@ -2547,7 +2540,7 @@
         <v>125</v>
       </c>
       <c r="B126" s="3" t="s">
-        <v>162</v>
+        <v>160</v>
       </c>
       <c r="C126" s="2" t="s">
         <v>150</v>
@@ -2689,12 +2682,12 @@
         <v>138</v>
       </c>
     </row>
-    <row r="138" spans="1:5" ht="45" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A138" s="2" t="s">
         <v>137</v>
       </c>
       <c r="B138" s="3" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="E138" s="2" t="s">
         <v>138</v>

</xml_diff>